<commit_message>
chore: rename pages to trigger sidebar menu
</commit_message>
<xml_diff>
--- a/data/transactions.xlsx
+++ b/data/transactions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanchuang/Desktop/資產計算/investment_tracker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanchuang/Desktop/資產計算/investment_tracker/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED48BFA2-FB0E-684B-BE35-F6E2FA357990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3232794-EE73-364F-8BD9-89B33F884776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1580" yWindow="1920" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="交易紀錄" sheetId="1" r:id="rId1"/>
@@ -639,16 +639,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L1005"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+      <selection activeCell="I253" sqref="I253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -699,7 +700,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>43774</v>
       </c>
@@ -735,7 +736,7 @@
         <v>78.374999999999986</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>43774</v>
       </c>
@@ -771,7 +772,7 @@
         <v>220.16249999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>43905</v>
       </c>
@@ -807,7 +808,7 @@
         <v>199.49999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>43994</v>
       </c>
@@ -848,7 +849,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>44020</v>
       </c>
@@ -884,7 +885,7 @@
         <v>247.66499999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>44040</v>
       </c>
@@ -920,7 +921,7 @@
         <v>330.59999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>44056</v>
       </c>
@@ -956,7 +957,7 @@
         <v>304.23749999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>44070</v>
       </c>
@@ -997,7 +998,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>44075</v>
       </c>
@@ -1033,7 +1034,7 @@
         <v>309.58124999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>44090</v>
       </c>
@@ -1074,7 +1075,7 @@
         <v>1378.5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>44091</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>319.2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>44165</v>
       </c>
@@ -1146,7 +1147,7 @@
         <v>346.27499999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>44181</v>
       </c>
@@ -1182,7 +1183,7 @@
         <v>504.44999999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>44183</v>
       </c>
@@ -1218,7 +1219,7 @@
         <v>499.46249999999992</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>44188</v>
       </c>
@@ -1259,7 +1260,7 @@
         <v>1060.8</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>44188</v>
       </c>
@@ -1300,7 +1301,7 @@
         <v>1524</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>44196</v>
       </c>
@@ -1336,7 +1337,7 @@
         <v>532.23749999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>44201</v>
       </c>
@@ -1377,7 +1378,7 @@
         <v>2355</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>44202</v>
       </c>
@@ -1413,7 +1414,7 @@
         <v>577.12499999999989</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>44204</v>
       </c>
@@ -1449,7 +1450,7 @@
         <v>413.24999999999994</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>44208</v>
       </c>
@@ -1485,7 +1486,7 @@
         <v>421.79999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>44209</v>
       </c>
@@ -1526,7 +1527,7 @@
         <v>2565</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>44209</v>
       </c>
@@ -1567,7 +1568,7 @@
         <v>2589</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>44209</v>
       </c>
@@ -1608,7 +1609,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>44210</v>
       </c>
@@ -1644,7 +1645,7 @@
         <v>424.65</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>44211</v>
       </c>
@@ -1752,7 +1753,7 @@
         <v>282.86249999999995</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
         <v>44217</v>
       </c>
@@ -1788,7 +1789,7 @@
         <v>454.57499999999993</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
         <v>44224</v>
       </c>
@@ -1947,7 +1948,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
         <v>44260</v>
       </c>
@@ -2019,7 +2020,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
         <v>44260</v>
       </c>
@@ -2055,7 +2056,7 @@
         <v>60.847499999999989</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
         <v>44286</v>
       </c>
@@ -2096,7 +2097,7 @@
         <v>3534</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11">
         <v>44286</v>
       </c>
@@ -2132,7 +2133,7 @@
         <v>839.32499999999993</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11">
         <v>44286</v>
       </c>
@@ -2168,7 +2169,7 @@
         <v>419.66249999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
         <v>44292</v>
       </c>
@@ -2204,7 +2205,7 @@
         <v>182.75624999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11">
         <v>44292</v>
       </c>
@@ -2276,7 +2277,7 @@
         <v>56.572499999999991</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
         <v>44293</v>
       </c>
@@ -2317,7 +2318,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
         <v>44294</v>
       </c>
@@ -2358,7 +2359,7 @@
         <v>820.5</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
         <v>44294</v>
       </c>
@@ -2435,7 +2436,7 @@
         <v>244.5</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11">
         <v>44295</v>
       </c>
@@ -2471,7 +2472,7 @@
         <v>102.24374999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="11">
         <v>44295</v>
       </c>
@@ -2507,7 +2508,7 @@
         <v>102.24374999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11">
         <v>44295</v>
       </c>
@@ -2543,7 +2544,7 @@
         <v>102.24374999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="11">
         <v>44298</v>
       </c>
@@ -2738,7 +2739,7 @@
         <v>61.41749999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11">
         <v>44299</v>
       </c>
@@ -2779,7 +2780,7 @@
         <v>439.5</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="11">
         <v>44300</v>
       </c>
@@ -2851,7 +2852,7 @@
         <v>59.992499999999993</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11">
         <v>44300</v>
       </c>
@@ -2887,7 +2888,7 @@
         <v>49.233749999999993</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11">
         <v>44301</v>
       </c>
@@ -2969,7 +2970,7 @@
         <v>262.5</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="11">
         <v>44306</v>
       </c>
@@ -3005,7 +3006,7 @@
         <v>49.304999999999993</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="11">
         <v>44306</v>
       </c>
@@ -3344,7 +3345,7 @@
         <v>32.276249999999997</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="11">
         <v>44329</v>
       </c>
@@ -3385,7 +3386,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="11">
         <v>44329</v>
       </c>
@@ -3426,7 +3427,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="11">
         <v>44329</v>
       </c>
@@ -3462,7 +3463,7 @@
         <v>81.224999999999994</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="11">
         <v>44329</v>
       </c>
@@ -3498,7 +3499,7 @@
         <v>81.937499999999986</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="11">
         <v>44329</v>
       </c>
@@ -3534,7 +3535,7 @@
         <v>391.87499999999994</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="11">
         <v>44329</v>
       </c>
@@ -3575,7 +3576,7 @@
         <v>349.5</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="11">
         <v>44329</v>
       </c>
@@ -3657,7 +3658,7 @@
         <v>209.1</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="11">
         <v>44330</v>
       </c>
@@ -3698,7 +3699,7 @@
         <v>457.2</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="11">
         <v>44333</v>
       </c>
@@ -3739,7 +3740,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="11">
         <v>44334</v>
       </c>
@@ -3775,7 +3776,7 @@
         <v>398.28749999999997</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11">
         <v>44334</v>
       </c>
@@ -3811,7 +3812,7 @@
         <v>398.28749999999997</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="11">
         <v>44337</v>
       </c>
@@ -3847,7 +3848,7 @@
         <v>75.524999999999991</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="11">
         <v>44337</v>
       </c>
@@ -3888,7 +3889,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="11">
         <v>44399</v>
       </c>
@@ -3929,7 +3930,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="11">
         <v>44399</v>
       </c>
@@ -3970,7 +3971,7 @@
         <v>589.5</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="11">
         <v>44406</v>
       </c>
@@ -4006,7 +4007,7 @@
         <v>411.82499999999993</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="11">
         <v>44407</v>
       </c>
@@ -4042,7 +4043,7 @@
         <v>194.65499999999997</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="11">
         <v>44407</v>
       </c>
@@ -4078,7 +4079,7 @@
         <v>27.431249999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="11">
         <v>44407</v>
       </c>
@@ -4114,7 +4115,7 @@
         <v>54.577499999999993</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="11">
         <v>44412</v>
       </c>
@@ -4150,7 +4151,7 @@
         <v>76.949999999999989</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="11">
         <v>44412</v>
       </c>
@@ -4186,7 +4187,7 @@
         <v>76.593749999999986</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="11">
         <v>44412</v>
       </c>
@@ -4227,7 +4228,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="11">
         <v>44412</v>
       </c>
@@ -4263,7 +4264,7 @@
         <v>52.938749999999992</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="11">
         <v>44412</v>
       </c>
@@ -4299,7 +4300,7 @@
         <v>79.728749999999977</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="11">
         <v>44412</v>
       </c>
@@ -4340,7 +4341,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="11">
         <v>44412</v>
       </c>
@@ -4376,7 +4377,7 @@
         <v>76.949999999999989</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="11">
         <v>44412</v>
       </c>
@@ -4412,7 +4413,7 @@
         <v>76.593749999999986</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="11">
         <v>44412</v>
       </c>
@@ -4448,7 +4449,7 @@
         <v>76.949999999999989</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="11">
         <v>44412</v>
       </c>
@@ -4484,7 +4485,7 @@
         <v>76.949999999999989</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="11">
         <v>44412</v>
       </c>
@@ -4520,7 +4521,7 @@
         <v>26.576249999999998</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="11">
         <v>44412</v>
       </c>
@@ -4556,7 +4557,7 @@
         <v>76.949999999999989</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="11">
         <v>44412</v>
       </c>
@@ -4592,7 +4593,7 @@
         <v>229.78124999999997</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="11">
         <v>44412</v>
       </c>
@@ -4628,7 +4629,7 @@
         <v>26.576249999999998</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="11">
         <v>44454</v>
       </c>
@@ -4669,7 +4670,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="11">
         <v>44454</v>
       </c>
@@ -4710,7 +4711,7 @@
         <v>255.9</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="11">
         <v>44462</v>
       </c>
@@ -4751,7 +4752,7 @@
         <v>352.5</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="11">
         <v>44462</v>
       </c>
@@ -4792,7 +4793,7 @@
         <v>355.5</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="11">
         <v>44462</v>
       </c>
@@ -4833,7 +4834,7 @@
         <v>1075.5</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="11">
         <v>44462</v>
       </c>
@@ -4874,7 +4875,7 @@
         <v>133.35</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="11">
         <v>44462</v>
       </c>
@@ -4915,7 +4916,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="11">
         <v>44462</v>
       </c>
@@ -4956,7 +4957,7 @@
         <v>134.55000000000001</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="11">
         <v>44466</v>
       </c>
@@ -4997,7 +4998,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="115" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="11">
         <v>44466</v>
       </c>
@@ -5038,7 +5039,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="116" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="11">
         <v>44473</v>
       </c>
@@ -5074,7 +5075,7 @@
         <v>406.83749999999998</v>
       </c>
     </row>
-    <row r="117" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="11">
         <v>44481</v>
       </c>
@@ -5115,7 +5116,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="118" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="11">
         <v>44484</v>
       </c>
@@ -5151,7 +5152,7 @@
         <v>388.31249999999994</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="11">
         <v>44490</v>
       </c>
@@ -5187,7 +5188,7 @@
         <v>123.11999999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="11">
         <v>44495</v>
       </c>
@@ -5228,7 +5229,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="11">
         <v>44529</v>
       </c>
@@ -5269,7 +5270,7 @@
         <v>560.70000000000005</v>
       </c>
     </row>
-    <row r="122" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="11">
         <v>44529</v>
       </c>
@@ -5310,7 +5311,7 @@
         <v>1791</v>
       </c>
     </row>
-    <row r="123" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="11">
         <v>44530</v>
       </c>
@@ -5346,7 +5347,7 @@
         <v>161.38124999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="11">
         <v>44530</v>
       </c>
@@ -5382,7 +5383,7 @@
         <v>136.79999999999998</v>
       </c>
     </row>
-    <row r="125" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="11">
         <v>44532</v>
       </c>
@@ -5418,7 +5419,7 @@
         <v>240.46874999999997</v>
       </c>
     </row>
-    <row r="126" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="11">
         <v>44533</v>
       </c>
@@ -5454,7 +5455,7 @@
         <v>279.65624999999994</v>
       </c>
     </row>
-    <row r="127" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="11">
         <v>44553</v>
       </c>
@@ -5495,7 +5496,7 @@
         <v>150.9</v>
       </c>
     </row>
-    <row r="128" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="11">
         <v>44554</v>
       </c>
@@ -5531,7 +5532,7 @@
         <v>35.197499999999998</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="11">
         <v>44557</v>
       </c>
@@ -5572,7 +5573,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="11">
         <v>44566</v>
       </c>
@@ -5608,7 +5609,7 @@
         <v>212.68124999999998</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="11">
         <v>44567</v>
       </c>
@@ -5644,7 +5645,7 @@
         <v>105.02249999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="11">
         <v>44568</v>
       </c>
@@ -5680,7 +5681,7 @@
         <v>89.774999999999991</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="11">
         <v>44586</v>
       </c>
@@ -5716,7 +5717,7 @@
         <v>100.81874999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="11">
         <v>44587</v>
       </c>
@@ -5752,7 +5753,7 @@
         <v>455.28749999999997</v>
       </c>
     </row>
-    <row r="135" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="11">
         <v>44587</v>
       </c>
@@ -5788,7 +5789,7 @@
         <v>100.99687499999999</v>
       </c>
     </row>
-    <row r="136" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="11">
         <v>44624</v>
       </c>
@@ -5829,7 +5830,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="137" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="11">
         <v>44638</v>
       </c>
@@ -5870,7 +5871,7 @@
         <v>388.5</v>
       </c>
     </row>
-    <row r="138" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="11">
         <v>44644</v>
       </c>
@@ -5906,7 +5907,7 @@
         <v>421.08749999999998</v>
       </c>
     </row>
-    <row r="139" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="11">
         <v>44650</v>
       </c>
@@ -5942,7 +5943,7 @@
         <v>426.07499999999993</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="11">
         <v>44652</v>
       </c>
@@ -5978,7 +5979,7 @@
         <v>416.81249999999994</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="11">
         <v>44658</v>
       </c>
@@ -6014,7 +6015,7 @@
         <v>406.83749999999998</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="11">
         <v>44753</v>
       </c>
@@ -6050,7 +6051,7 @@
         <v>160.31249999999997</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="11">
         <v>44753</v>
       </c>
@@ -6086,7 +6087,7 @@
         <v>160.16999999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="11">
         <v>44812</v>
       </c>
@@ -6122,7 +6123,7 @@
         <v>160.88249999999999</v>
       </c>
     </row>
-    <row r="145" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="11">
         <v>44838</v>
       </c>
@@ -6163,7 +6164,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="146" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="11">
         <v>44848</v>
       </c>
@@ -6199,7 +6200,7 @@
         <v>294.26249999999999</v>
       </c>
     </row>
-    <row r="147" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="11">
         <v>44848</v>
       </c>
@@ -6235,7 +6236,7 @@
         <v>72.674999999999997</v>
       </c>
     </row>
-    <row r="148" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="11">
         <v>44883</v>
       </c>
@@ -6276,7 +6277,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="149" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="11">
         <v>44897</v>
       </c>
@@ -6312,7 +6313,7 @@
         <v>130.52999999999997</v>
       </c>
     </row>
-    <row r="150" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="11">
         <v>44900</v>
       </c>
@@ -6348,7 +6349,7 @@
         <v>341.99999999999994</v>
       </c>
     </row>
-    <row r="151" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="11">
         <v>44902</v>
       </c>
@@ -6384,7 +6385,7 @@
         <v>350.54999999999995</v>
       </c>
     </row>
-    <row r="152" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="11">
         <v>44902</v>
       </c>
@@ -6420,7 +6421,7 @@
         <v>76.949999999999989</v>
       </c>
     </row>
-    <row r="153" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="11">
         <v>45009</v>
       </c>
@@ -6461,7 +6462,7 @@
         <v>1567.5</v>
       </c>
     </row>
-    <row r="154" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="11">
         <v>45117</v>
       </c>
@@ -6497,7 +6498,7 @@
         <v>273.27937499999996</v>
       </c>
     </row>
-    <row r="155" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="11">
         <v>45120</v>
       </c>
@@ -6538,7 +6539,7 @@
         <v>1196.6400000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="11">
         <v>45139</v>
       </c>
@@ -6574,7 +6575,7 @@
         <v>276.69937499999992</v>
       </c>
     </row>
-    <row r="157" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="11">
         <v>45148</v>
       </c>
@@ -6610,7 +6611,7 @@
         <v>394.01249999999993</v>
       </c>
     </row>
-    <row r="158" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="11">
         <v>45154</v>
       </c>
@@ -6646,7 +6647,7 @@
         <v>384.74999999999994</v>
       </c>
     </row>
-    <row r="159" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="11">
         <v>45160</v>
       </c>
@@ -6682,7 +6683,7 @@
         <v>176.41499999999999</v>
       </c>
     </row>
-    <row r="160" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="11">
         <v>45232</v>
       </c>
@@ -6718,7 +6719,7 @@
         <v>88.35</v>
       </c>
     </row>
-    <row r="161" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="11">
         <v>45263</v>
       </c>
@@ -6754,7 +6755,7 @@
         <v>132.92399999999998</v>
       </c>
     </row>
-    <row r="162" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="11">
         <v>45294</v>
       </c>
@@ -6795,7 +6796,7 @@
         <v>628.80000000000007</v>
       </c>
     </row>
-    <row r="163" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="11">
         <v>45310</v>
       </c>
@@ -6831,7 +6832,7 @@
         <v>298.67999999999995</v>
       </c>
     </row>
-    <row r="164" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="11">
         <v>45344</v>
       </c>
@@ -6867,7 +6868,7 @@
         <v>492.33749999999992</v>
       </c>
     </row>
-    <row r="165" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="11">
         <v>45362</v>
       </c>
@@ -6908,7 +6909,7 @@
         <v>1591.2</v>
       </c>
     </row>
-    <row r="166" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="11">
         <v>45363</v>
       </c>
@@ -6944,7 +6945,7 @@
         <v>547.91249999999991</v>
       </c>
     </row>
-    <row r="167" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="11">
         <v>45389</v>
       </c>
@@ -6980,7 +6981,7 @@
         <v>28.001249999999995</v>
       </c>
     </row>
-    <row r="168" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="11">
         <v>45389</v>
       </c>
@@ -7016,7 +7017,7 @@
         <v>118.91624999999999</v>
       </c>
     </row>
-    <row r="169" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="11">
         <v>45389</v>
       </c>
@@ -7052,7 +7053,7 @@
         <v>122.79937499999998</v>
       </c>
     </row>
-    <row r="170" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="11">
         <v>45389</v>
       </c>
@@ -7088,7 +7089,7 @@
         <v>105.84187499999999</v>
       </c>
     </row>
-    <row r="171" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="11">
         <v>45397</v>
       </c>
@@ -7129,7 +7130,7 @@
         <v>4830</v>
       </c>
     </row>
-    <row r="172" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="11">
         <v>45397</v>
       </c>
@@ -7170,7 +7171,7 @@
         <v>14490</v>
       </c>
     </row>
-    <row r="173" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="11">
         <v>45401</v>
       </c>
@@ -7206,7 +7207,7 @@
         <v>1075.8749999999998</v>
       </c>
     </row>
-    <row r="174" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="11">
         <v>45405</v>
       </c>
@@ -7242,7 +7243,7 @@
         <v>537.93749999999989</v>
       </c>
     </row>
-    <row r="175" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="11">
         <v>45411</v>
       </c>
@@ -7278,7 +7279,7 @@
         <v>562.87499999999989</v>
       </c>
     </row>
-    <row r="176" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="11">
         <v>45412</v>
       </c>
@@ -7314,7 +7315,7 @@
         <v>1139.9999999999998</v>
       </c>
     </row>
-    <row r="177" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="11">
         <v>45414</v>
       </c>
@@ -7350,7 +7351,7 @@
         <v>555.74999999999989</v>
       </c>
     </row>
-    <row r="178" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="11">
         <v>45418</v>
       </c>
@@ -7386,7 +7387,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="179" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="11">
         <v>45475</v>
       </c>
@@ -7420,7 +7421,7 @@
       </c>
       <c r="K179" s="10"/>
     </row>
-    <row r="180" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="11">
         <v>45475</v>
       </c>
@@ -7454,7 +7455,7 @@
       </c>
       <c r="K180" s="10"/>
     </row>
-    <row r="181" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="11">
         <v>45475</v>
       </c>
@@ -7488,7 +7489,7 @@
       </c>
       <c r="K181" s="10"/>
     </row>
-    <row r="182" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="11">
         <v>45475</v>
       </c>
@@ -7522,7 +7523,7 @@
       </c>
       <c r="K182" s="10"/>
     </row>
-    <row r="183" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="11">
         <v>45475</v>
       </c>
@@ -7556,7 +7557,7 @@
       </c>
       <c r="K183" s="10"/>
     </row>
-    <row r="184" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="11">
         <v>45476</v>
       </c>
@@ -7590,7 +7591,7 @@
       </c>
       <c r="K184" s="10"/>
     </row>
-    <row r="185" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="11">
         <v>45476</v>
       </c>
@@ -7631,7 +7632,7 @@
         <v>406.5</v>
       </c>
     </row>
-    <row r="186" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="11">
         <v>45476</v>
       </c>
@@ -7672,7 +7673,7 @@
         <v>569.1</v>
       </c>
     </row>
-    <row r="187" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="11">
         <v>45476</v>
       </c>
@@ -7706,7 +7707,7 @@
       </c>
       <c r="K187" s="10"/>
     </row>
-    <row r="188" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="11">
         <v>45476</v>
       </c>
@@ -7740,7 +7741,7 @@
       </c>
       <c r="K188" s="10"/>
     </row>
-    <row r="189" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="11">
         <v>45488</v>
       </c>
@@ -7781,7 +7782,7 @@
         <v>24720</v>
       </c>
     </row>
-    <row r="190" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="11">
         <v>45489</v>
       </c>
@@ -7817,7 +7818,7 @@
         <v>6098.9999999999991</v>
       </c>
     </row>
-    <row r="191" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="11">
         <v>45489</v>
       </c>
@@ -7851,7 +7852,7 @@
       </c>
       <c r="K191" s="10"/>
     </row>
-    <row r="192" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="11">
         <v>45489</v>
       </c>
@@ -7885,7 +7886,7 @@
       </c>
       <c r="K192" s="10"/>
     </row>
-    <row r="193" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="11">
         <v>45489</v>
       </c>
@@ -7919,7 +7920,7 @@
       </c>
       <c r="K193" s="10"/>
     </row>
-    <row r="194" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="11">
         <v>45490</v>
       </c>
@@ -7953,7 +7954,7 @@
       </c>
       <c r="K194" s="10"/>
     </row>
-    <row r="195" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="11">
         <v>45490</v>
       </c>
@@ -7987,7 +7988,7 @@
       </c>
       <c r="K195" s="10"/>
     </row>
-    <row r="196" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="11">
         <v>45490</v>
       </c>
@@ -8021,7 +8022,7 @@
       </c>
       <c r="K196" s="10"/>
     </row>
-    <row r="197" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="11">
         <v>45490</v>
       </c>
@@ -8055,7 +8056,7 @@
       </c>
       <c r="K197" s="10"/>
     </row>
-    <row r="198" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="11">
         <v>45492</v>
       </c>
@@ -8089,7 +8090,7 @@
       </c>
       <c r="K198" s="10"/>
     </row>
-    <row r="199" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="11">
         <v>45492</v>
       </c>
@@ -8123,7 +8124,7 @@
       </c>
       <c r="K199" s="10"/>
     </row>
-    <row r="200" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="11">
         <v>45492</v>
       </c>
@@ -8157,7 +8158,7 @@
       </c>
       <c r="K200" s="10"/>
     </row>
-    <row r="201" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="11">
         <v>45506</v>
       </c>
@@ -8198,7 +8199,7 @@
         <v>534.29999999999995</v>
       </c>
     </row>
-    <row r="202" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="11">
         <v>45506</v>
       </c>
@@ -8234,7 +8235,7 @@
         <v>647.66249999999991</v>
       </c>
     </row>
-    <row r="203" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="11">
         <v>45506</v>
       </c>
@@ -8275,7 +8276,7 @@
         <v>488.55</v>
       </c>
     </row>
-    <row r="204" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="11">
         <v>45506</v>
       </c>
@@ -8316,7 +8317,7 @@
         <v>543.75</v>
       </c>
     </row>
-    <row r="205" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="11">
         <v>45506</v>
       </c>
@@ -8357,7 +8358,7 @@
         <v>137.85</v>
       </c>
     </row>
-    <row r="206" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="11">
         <v>45509</v>
       </c>
@@ -8393,7 +8394,7 @@
         <v>117.27749999999999</v>
       </c>
     </row>
-    <row r="207" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="11">
         <v>45510</v>
       </c>
@@ -8427,7 +8428,7 @@
       </c>
       <c r="K207" s="10"/>
     </row>
-    <row r="208" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="11">
         <v>45510</v>
       </c>
@@ -8461,7 +8462,7 @@
       </c>
       <c r="K208" s="10"/>
     </row>
-    <row r="209" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="11">
         <v>45511</v>
       </c>
@@ -8495,7 +8496,7 @@
       </c>
       <c r="K209" s="10"/>
     </row>
-    <row r="210" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="11">
         <v>45511</v>
       </c>
@@ -8529,7 +8530,7 @@
       </c>
       <c r="K210" s="10"/>
     </row>
-    <row r="211" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="11">
         <v>45511</v>
       </c>
@@ -8563,7 +8564,7 @@
       </c>
       <c r="K211" s="10"/>
     </row>
-    <row r="212" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="11">
         <v>45533</v>
       </c>
@@ -8597,7 +8598,7 @@
       </c>
       <c r="K212" s="10"/>
     </row>
-    <row r="213" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="11">
         <v>45533</v>
       </c>
@@ -8631,7 +8632,7 @@
       </c>
       <c r="K213" s="10"/>
     </row>
-    <row r="214" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="11">
         <v>45533</v>
       </c>
@@ -8665,7 +8666,7 @@
       </c>
       <c r="K214" s="10"/>
     </row>
-    <row r="215" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="11">
         <v>45533</v>
       </c>
@@ -8699,7 +8700,7 @@
       </c>
       <c r="K215" s="10"/>
     </row>
-    <row r="216" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="11">
         <v>45546</v>
       </c>
@@ -8733,7 +8734,7 @@
       </c>
       <c r="K216" s="10"/>
     </row>
-    <row r="217" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="11">
         <v>45546</v>
       </c>
@@ -8767,7 +8768,7 @@
       </c>
       <c r="K217" s="10"/>
     </row>
-    <row r="218" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="11">
         <v>45559</v>
       </c>
@@ -8801,7 +8802,7 @@
       </c>
       <c r="K218" s="10"/>
     </row>
-    <row r="219" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="11">
         <v>45581</v>
       </c>
@@ -8835,7 +8836,7 @@
       </c>
       <c r="K219" s="10"/>
     </row>
-    <row r="220" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="11">
         <v>45607</v>
       </c>
@@ -8869,7 +8870,7 @@
       </c>
       <c r="K220" s="10"/>
     </row>
-    <row r="221" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="11">
         <v>45607</v>
       </c>
@@ -8903,7 +8904,7 @@
       </c>
       <c r="K221" s="10"/>
     </row>
-    <row r="222" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="11">
         <v>45614</v>
       </c>
@@ -8937,7 +8938,7 @@
       </c>
       <c r="K222" s="10"/>
     </row>
-    <row r="223" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="11">
         <v>45614</v>
       </c>
@@ -8971,7 +8972,7 @@
       </c>
       <c r="K223" s="10"/>
     </row>
-    <row r="224" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="11">
         <v>45614</v>
       </c>
@@ -9005,7 +9006,7 @@
       </c>
       <c r="K224" s="10"/>
     </row>
-    <row r="225" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="11">
         <v>45614</v>
       </c>
@@ -9039,7 +9040,7 @@
       </c>
       <c r="K225" s="10"/>
     </row>
-    <row r="226" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="11">
         <v>45645</v>
       </c>
@@ -9080,7 +9081,7 @@
         <v>3210</v>
       </c>
     </row>
-    <row r="227" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="11">
         <v>45645</v>
       </c>
@@ -9114,7 +9115,7 @@
       </c>
       <c r="K227" s="10"/>
     </row>
-    <row r="228" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="11">
         <v>45645</v>
       </c>
@@ -9148,7 +9149,7 @@
       </c>
       <c r="K228" s="10"/>
     </row>
-    <row r="229" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="11">
         <v>45649</v>
       </c>
@@ -9182,7 +9183,7 @@
       </c>
       <c r="K229" s="10"/>
     </row>
-    <row r="230" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="11">
         <v>45649</v>
       </c>
@@ -9216,7 +9217,7 @@
       </c>
       <c r="K230" s="10"/>
     </row>
-    <row r="231" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="11">
         <v>45649</v>
       </c>
@@ -9250,7 +9251,7 @@
       </c>
       <c r="K231" s="10"/>
     </row>
-    <row r="232" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="11">
         <v>45649</v>
       </c>
@@ -9284,7 +9285,7 @@
       </c>
       <c r="K232" s="10"/>
     </row>
-    <row r="233" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="11">
         <v>45691</v>
       </c>
@@ -9318,7 +9319,7 @@
       </c>
       <c r="K233" s="10"/>
     </row>
-    <row r="234" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="11">
         <v>45691</v>
       </c>
@@ -9352,7 +9353,7 @@
       </c>
       <c r="K234" s="10"/>
     </row>
-    <row r="235" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="11">
         <v>45691</v>
       </c>
@@ -9386,7 +9387,7 @@
       </c>
       <c r="K235" s="10"/>
     </row>
-    <row r="236" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="11">
         <v>45719</v>
       </c>
@@ -9420,7 +9421,7 @@
       </c>
       <c r="K236" s="10"/>
     </row>
-    <row r="237" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="11">
         <v>45720</v>
       </c>
@@ -9454,7 +9455,7 @@
       </c>
       <c r="K237" s="10"/>
     </row>
-    <row r="238" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="11">
         <v>45726</v>
       </c>
@@ -9488,7 +9489,7 @@
       </c>
       <c r="K238" s="10"/>
     </row>
-    <row r="239" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="11">
         <v>45726</v>
       </c>
@@ -9522,7 +9523,7 @@
       </c>
       <c r="K239" s="10"/>
     </row>
-    <row r="240" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="11">
         <v>45726</v>
       </c>
@@ -9556,7 +9557,7 @@
       </c>
       <c r="K240" s="10"/>
     </row>
-    <row r="241" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="11">
         <v>45728</v>
       </c>
@@ -9590,7 +9591,7 @@
       </c>
       <c r="K241" s="10"/>
     </row>
-    <row r="242" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="11">
         <v>45727</v>
       </c>
@@ -9631,7 +9632,7 @@
         <v>2910</v>
       </c>
     </row>
-    <row r="243" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="11">
         <v>45728</v>
       </c>
@@ -9665,7 +9666,7 @@
       </c>
       <c r="K243" s="10"/>
     </row>
-    <row r="244" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="11">
         <v>45747</v>
       </c>
@@ -9701,7 +9702,7 @@
         <v>648.37499999999989</v>
       </c>
     </row>
-    <row r="245" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="11">
         <v>45755</v>
       </c>
@@ -9737,7 +9738,7 @@
         <v>577.12499999999989</v>
       </c>
     </row>
-    <row r="246" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="11">
         <v>45758</v>
       </c>
@@ -12152,7 +12153,17 @@
       <c r="H1005" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L246" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L246" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="2002"/>
+        <filter val="2338"/>
+        <filter val="4938"/>
+        <filter val="6278"/>
+        <filter val="6414"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D89" r:id="rId1" display="6770.TW" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
調整 bar_chart 的 tooltip 顯示：index -> date, color -> stock
</commit_message>
<xml_diff>
--- a/data/transactions.xlsx
+++ b/data/transactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanchuang/Desktop/資產計算/investment_tracker/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BFB8B4-27F9-9546-AA7E-7B5094633B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF473E3-7C4B-A546-9A8A-A76767020055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="交易紀錄" sheetId="1" r:id="rId1"/>
@@ -641,7 +641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <selection activeCell="E227" sqref="E227"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
🎯 Major Update: Refactored holdings & cash summary, improved USD split logic, added visual charts, and introduced animated Asset Monster homepage
</commit_message>
<xml_diff>
--- a/data/transactions.xlsx
+++ b/data/transactions.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanchuang/Desktop/資產計算/investment_tracker/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4228A649-98C2-8348-86A2-B679BA6F5397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCF7E63-B77B-8F48-9782-9DE809CB87F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="交易主表" sheetId="1" r:id="rId1"/>
     <sheet name="出資比例" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">交易主表!$A$1:$M$246</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">交易主表!$A$1:$M$245</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2334" uniqueCount="322">
   <si>
     <t>交易日期</t>
   </si>
@@ -975,9 +975,6 @@
   </si>
   <si>
     <t>TX00240</t>
-  </si>
-  <si>
-    <t>TX00241</t>
   </si>
   <si>
     <t>TX00242</t>
@@ -1418,10 +1415,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:M246"/>
+  <dimension ref="A1:M245"/>
   <sheetViews>
     <sheetView zoomScale="186" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A243" sqref="A243:XFD243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2736,7 +2733,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" hidden="1">
       <c r="A35" s="2">
         <v>44260</v>
       </c>
@@ -6688,7 +6685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:12">
+    <row r="139" spans="1:12" hidden="1">
       <c r="A139" s="2">
         <v>44650</v>
       </c>
@@ -6726,7 +6723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:12">
+    <row r="140" spans="1:12" hidden="1">
       <c r="A140" s="2">
         <v>44652</v>
       </c>
@@ -6764,7 +6761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:12">
+    <row r="141" spans="1:12" hidden="1">
       <c r="A141" s="2">
         <v>44658</v>
       </c>
@@ -6954,7 +6951,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="146" spans="1:12">
+    <row r="146" spans="1:12" hidden="1">
       <c r="A146" s="2">
         <v>44848</v>
       </c>
@@ -6992,7 +6989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:12">
+    <row r="147" spans="1:12" hidden="1">
       <c r="A147" s="2">
         <v>44848</v>
       </c>
@@ -7030,7 +7027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:12">
+    <row r="148" spans="1:12" hidden="1">
       <c r="A148" s="2">
         <v>44883</v>
       </c>
@@ -7106,7 +7103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:12">
+    <row r="150" spans="1:12" hidden="1">
       <c r="A150" s="2">
         <v>44900</v>
       </c>
@@ -7638,7 +7635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:12">
+    <row r="164" spans="1:12" hidden="1">
       <c r="A164" s="2">
         <v>45344</v>
       </c>
@@ -8208,7 +8205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:12">
+    <row r="179" spans="1:12" hidden="1">
       <c r="A179" s="2">
         <v>45475</v>
       </c>
@@ -8284,7 +8281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:12">
+    <row r="181" spans="1:12" hidden="1">
       <c r="A181" s="2">
         <v>45475</v>
       </c>
@@ -8322,7 +8319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:12">
+    <row r="182" spans="1:12" hidden="1">
       <c r="A182" s="2">
         <v>45475</v>
       </c>
@@ -8512,7 +8509,7 @@
         <v>569.1</v>
       </c>
     </row>
-    <row r="187" spans="1:12">
+    <row r="187" spans="1:12" hidden="1">
       <c r="A187" s="2">
         <v>45476</v>
       </c>
@@ -8550,7 +8547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:12">
+    <row r="188" spans="1:12" hidden="1">
       <c r="A188" s="2">
         <v>45476</v>
       </c>
@@ -8664,7 +8661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:12">
+    <row r="191" spans="1:12" hidden="1">
       <c r="A191" s="2">
         <v>45489</v>
       </c>
@@ -8702,7 +8699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:12">
+    <row r="192" spans="1:12" hidden="1">
       <c r="A192" s="2">
         <v>45489</v>
       </c>
@@ -8778,7 +8775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:12">
+    <row r="194" spans="1:12" hidden="1">
       <c r="A194" s="2">
         <v>45490</v>
       </c>
@@ -8816,7 +8813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:12">
+    <row r="195" spans="1:12" hidden="1">
       <c r="A195" s="2">
         <v>45490</v>
       </c>
@@ -8854,7 +8851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:12">
+    <row r="196" spans="1:12" hidden="1">
       <c r="A196" s="2">
         <v>45490</v>
       </c>
@@ -8892,7 +8889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:12">
+    <row r="197" spans="1:12" hidden="1">
       <c r="A197" s="2">
         <v>45490</v>
       </c>
@@ -8930,7 +8927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:12">
+    <row r="198" spans="1:12" hidden="1">
       <c r="A198" s="2">
         <v>45492</v>
       </c>
@@ -8968,7 +8965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:12">
+    <row r="199" spans="1:12" hidden="1">
       <c r="A199" s="2">
         <v>45492</v>
       </c>
@@ -9006,7 +9003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:12">
+    <row r="200" spans="1:12" hidden="1">
       <c r="A200" s="2">
         <v>45492</v>
       </c>
@@ -9272,7 +9269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:12">
+    <row r="207" spans="1:12" hidden="1">
       <c r="A207" s="2">
         <v>45510</v>
       </c>
@@ -9310,7 +9307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:12">
+    <row r="208" spans="1:12" hidden="1">
       <c r="A208" s="2">
         <v>45510</v>
       </c>
@@ -9348,7 +9345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:12">
+    <row r="209" spans="1:12" hidden="1">
       <c r="A209" s="2">
         <v>45511</v>
       </c>
@@ -9386,7 +9383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:12">
+    <row r="210" spans="1:12" hidden="1">
       <c r="A210" s="2">
         <v>45511</v>
       </c>
@@ -9424,7 +9421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:12">
+    <row r="211" spans="1:12" hidden="1">
       <c r="A211" s="2">
         <v>45511</v>
       </c>
@@ -9462,7 +9459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:12">
+    <row r="212" spans="1:12" hidden="1">
       <c r="A212" s="2">
         <v>45533</v>
       </c>
@@ -9500,7 +9497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:12">
+    <row r="213" spans="1:12" hidden="1">
       <c r="A213" s="2">
         <v>45533</v>
       </c>
@@ -9538,7 +9535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:12">
+    <row r="214" spans="1:12" hidden="1">
       <c r="A214" s="2">
         <v>45533</v>
       </c>
@@ -9576,7 +9573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:12">
+    <row r="215" spans="1:12" hidden="1">
       <c r="A215" s="2">
         <v>45533</v>
       </c>
@@ -9614,7 +9611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:12">
+    <row r="216" spans="1:12" hidden="1">
       <c r="A216" s="2">
         <v>45546</v>
       </c>
@@ -9652,7 +9649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:12">
+    <row r="217" spans="1:12" hidden="1">
       <c r="A217" s="2">
         <v>45546</v>
       </c>
@@ -9690,7 +9687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:12">
+    <row r="218" spans="1:12" hidden="1">
       <c r="A218" s="2">
         <v>45559</v>
       </c>
@@ -9728,7 +9725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:12">
+    <row r="219" spans="1:12" hidden="1">
       <c r="A219" s="2">
         <v>45581</v>
       </c>
@@ -9956,7 +9953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:12">
+    <row r="225" spans="1:12" hidden="1">
       <c r="A225" s="2">
         <v>45614</v>
       </c>
@@ -10108,7 +10105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:12">
+    <row r="229" spans="1:12" hidden="1">
       <c r="A229" s="2">
         <v>45649</v>
       </c>
@@ -10260,7 +10257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:12">
+    <row r="233" spans="1:12" hidden="1">
       <c r="A233" s="2">
         <v>45691</v>
       </c>
@@ -10298,7 +10295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:12">
+    <row r="234" spans="1:12" hidden="1">
       <c r="A234" s="2">
         <v>45691</v>
       </c>
@@ -10336,7 +10333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:12">
+    <row r="235" spans="1:12" hidden="1">
       <c r="A235" s="2">
         <v>45691</v>
       </c>
@@ -10374,7 +10371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:12">
+    <row r="236" spans="1:12" hidden="1">
       <c r="A236" s="2">
         <v>45719</v>
       </c>
@@ -10640,39 +10637,39 @@
         <v>2910</v>
       </c>
     </row>
-    <row r="243" spans="1:12">
+    <row r="243" spans="1:12" hidden="1">
       <c r="A243" s="2">
-        <v>45728</v>
+        <v>45747</v>
       </c>
       <c r="B243" s="3" t="s">
         <v>317</v>
       </c>
       <c r="C243" s="3" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="D243" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E243" s="3" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="F243" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G243" s="3" t="s">
         <v>71</v>
       </c>
       <c r="H243" s="3">
-        <v>247.34989999999999</v>
+        <v>910</v>
       </c>
       <c r="I243" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J243" s="3">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="K243" s="6">
-        <v>0</v>
+        <v>648.37499999999989</v>
       </c>
       <c r="L243" s="6">
         <v>0</v>
@@ -10680,7 +10677,7 @@
     </row>
     <row r="244" spans="1:12" hidden="1">
       <c r="A244" s="2">
-        <v>45747</v>
+        <v>45755</v>
       </c>
       <c r="B244" s="3" t="s">
         <v>318</v>
@@ -10701,7 +10698,7 @@
         <v>71</v>
       </c>
       <c r="H244" s="3">
-        <v>910</v>
+        <v>810</v>
       </c>
       <c r="I244" s="3" t="s">
         <v>74</v>
@@ -10710,7 +10707,7 @@
         <v>1000</v>
       </c>
       <c r="K244" s="6">
-        <v>648.37499999999989</v>
+        <v>577.12499999999989</v>
       </c>
       <c r="L244" s="6">
         <v>0</v>
@@ -10718,7 +10715,7 @@
     </row>
     <row r="245" spans="1:12" hidden="1">
       <c r="A245" s="2">
-        <v>45755</v>
+        <v>45758</v>
       </c>
       <c r="B245" s="3" t="s">
         <v>319</v>
@@ -10736,64 +10733,31 @@
         <v>69</v>
       </c>
       <c r="G245" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H245" s="3">
-        <v>810</v>
+        <v>880</v>
       </c>
       <c r="I245" s="3" t="s">
         <v>74</v>
       </c>
       <c r="J245" s="3">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="K245" s="6">
-        <v>577.12499999999989</v>
+        <v>-626.99999999999989</v>
       </c>
       <c r="L245" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="1:12" hidden="1">
-      <c r="A246" s="2">
-        <v>45758</v>
-      </c>
-      <c r="B246" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="C246" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D246" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E246" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F246" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G246" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H246" s="3">
-        <v>880</v>
-      </c>
-      <c r="I246" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J246" s="3">
-        <v>-1000</v>
-      </c>
-      <c r="K246" s="6">
-        <v>-626.99999999999989</v>
-      </c>
-      <c r="L246" s="6">
         <v>2640</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M246" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:M245" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="TSLA"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="8">
       <filters>
         <filter val="Joint"/>
@@ -10807,10 +10771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C308"/>
+  <dimension ref="A1:C306"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
+      <selection activeCell="A317" sqref="A317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -10823,10 +10787,10 @@
         <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>321</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -14159,50 +14123,28 @@
         <v>74</v>
       </c>
       <c r="C304" s="1">
-        <v>0.65200000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="305" spans="1:3">
       <c r="A305" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C305" s="1">
-        <v>0.34799999999999998</v>
+        <v>1</v>
       </c>
     </row>
     <row r="306" spans="1:3">
       <c r="A306" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B306" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C306" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="307" spans="1:3">
-      <c r="A307" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="B307" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C307" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="308" spans="1:3">
-      <c r="A308" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="B308" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C308" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add expand_joint_transactions_by_ownership() to split Joint transactions by ownership
</commit_message>
<xml_diff>
--- a/data/transactions.xlsx
+++ b/data/transactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanchuang/Desktop/資產計算/investment_tracker/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCF7E63-B77B-8F48-9782-9DE809CB87F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A38E055-B6CC-6844-B021-108B5040965B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="交易主表" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2334" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2335" uniqueCount="323">
   <si>
     <t>交易日期</t>
   </si>
@@ -990,6 +990,10 @@
   </si>
   <si>
     <t>出資比例</t>
+  </si>
+  <si>
+    <t>第一筆太早了不可考</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -999,7 +1003,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1034,6 +1038,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF506A86"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
@@ -1096,7 +1108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1110,6 +1122,8 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1414,11 +1428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:M245"/>
   <sheetViews>
-    <sheetView zoomScale="186" workbookViewId="0">
-      <selection activeCell="A243" sqref="A243:XFD243"/>
+    <sheetView tabSelected="1" zoomScale="186" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1479,9 +1492,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1">
-      <c r="A2" s="2">
-        <v>43774</v>
+    <row r="2" spans="1:13">
+      <c r="A2" s="7">
+        <v>43770</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>76</v>
@@ -1516,8 +1529,11 @@
       <c r="L2" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" hidden="1">
+      <c r="M2" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="2">
         <v>43774</v>
       </c>
@@ -1555,7 +1571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1">
+    <row r="4" spans="1:13">
       <c r="A4" s="2">
         <v>43905</v>
       </c>
@@ -1593,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1">
+    <row r="5" spans="1:13">
       <c r="A5" s="2">
         <v>43994</v>
       </c>
@@ -1631,7 +1647,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1">
+    <row r="6" spans="1:13">
       <c r="A6" s="2">
         <v>44020</v>
       </c>
@@ -1669,7 +1685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1">
+    <row r="7" spans="1:13">
       <c r="A7" s="2">
         <v>44040</v>
       </c>
@@ -1707,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1">
+    <row r="8" spans="1:13">
       <c r="A8" s="2">
         <v>44056</v>
       </c>
@@ -1745,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1">
+    <row r="9" spans="1:13">
       <c r="A9" s="2">
         <v>44070</v>
       </c>
@@ -1783,7 +1799,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1">
+    <row r="10" spans="1:13">
       <c r="A10" s="2">
         <v>44075</v>
       </c>
@@ -1821,7 +1837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1">
+    <row r="11" spans="1:13">
       <c r="A11" s="2">
         <v>44090</v>
       </c>
@@ -1859,7 +1875,7 @@
         <v>1378.5</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1">
+    <row r="12" spans="1:13">
       <c r="A12" s="2">
         <v>44091</v>
       </c>
@@ -1897,7 +1913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1">
+    <row r="13" spans="1:13">
       <c r="A13" s="2">
         <v>44165</v>
       </c>
@@ -1935,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1">
+    <row r="14" spans="1:13">
       <c r="A14" s="2">
         <v>44181</v>
       </c>
@@ -1973,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1">
+    <row r="15" spans="1:13">
       <c r="A15" s="2">
         <v>44183</v>
       </c>
@@ -2011,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1">
+    <row r="16" spans="1:13">
       <c r="A16" s="2">
         <v>44188</v>
       </c>
@@ -2049,7 +2065,7 @@
         <v>1060.8</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1">
+    <row r="17" spans="1:12">
       <c r="A17" s="2">
         <v>44188</v>
       </c>
@@ -2087,7 +2103,7 @@
         <v>1524</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1">
+    <row r="18" spans="1:12">
       <c r="A18" s="2">
         <v>44196</v>
       </c>
@@ -2125,7 +2141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1">
+    <row r="19" spans="1:12">
       <c r="A19" s="2">
         <v>44201</v>
       </c>
@@ -2163,7 +2179,7 @@
         <v>2355</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1">
+    <row r="20" spans="1:12">
       <c r="A20" s="2">
         <v>44202</v>
       </c>
@@ -2201,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1">
+    <row r="21" spans="1:12">
       <c r="A21" s="2">
         <v>44204</v>
       </c>
@@ -2239,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1">
+    <row r="22" spans="1:12">
       <c r="A22" s="2">
         <v>44208</v>
       </c>
@@ -2277,7 +2293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1">
+    <row r="23" spans="1:12">
       <c r="A23" s="2">
         <v>44209</v>
       </c>
@@ -2315,7 +2331,7 @@
         <v>2565</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1">
+    <row r="24" spans="1:12">
       <c r="A24" s="2">
         <v>44209</v>
       </c>
@@ -2353,7 +2369,7 @@
         <v>2589</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1">
+    <row r="25" spans="1:12">
       <c r="A25" s="2">
         <v>44209</v>
       </c>
@@ -2391,7 +2407,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1">
+    <row r="26" spans="1:12">
       <c r="A26" s="2">
         <v>44210</v>
       </c>
@@ -2429,7 +2445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1">
+    <row r="27" spans="1:12">
       <c r="A27" s="2">
         <v>44211</v>
       </c>
@@ -2467,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1">
+    <row r="28" spans="1:12">
       <c r="A28" s="2">
         <v>44215</v>
       </c>
@@ -2505,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1">
+    <row r="29" spans="1:12">
       <c r="A29" s="2">
         <v>44215</v>
       </c>
@@ -2543,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1">
+    <row r="30" spans="1:12">
       <c r="A30" s="2">
         <v>44217</v>
       </c>
@@ -2581,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1">
+    <row r="31" spans="1:12">
       <c r="A31" s="2">
         <v>44224</v>
       </c>
@@ -2619,7 +2635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1">
+    <row r="32" spans="1:12">
       <c r="A32" s="2">
         <v>44224</v>
       </c>
@@ -2657,7 +2673,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1">
+    <row r="33" spans="1:12">
       <c r="A33" s="2">
         <v>44224</v>
       </c>
@@ -2695,7 +2711,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1">
+    <row r="34" spans="1:12">
       <c r="A34" s="2">
         <v>44260</v>
       </c>
@@ -2733,7 +2749,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1">
+    <row r="35" spans="1:12">
       <c r="A35" s="2">
         <v>44260</v>
       </c>
@@ -2771,7 +2787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1">
+    <row r="36" spans="1:12">
       <c r="A36" s="2">
         <v>44260</v>
       </c>
@@ -2809,7 +2825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1">
+    <row r="37" spans="1:12">
       <c r="A37" s="2">
         <v>44260</v>
       </c>
@@ -2847,7 +2863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1">
+    <row r="38" spans="1:12">
       <c r="A38" s="2">
         <v>44286</v>
       </c>
@@ -2885,7 +2901,7 @@
         <v>3534</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1">
+    <row r="39" spans="1:12">
       <c r="A39" s="2">
         <v>44286</v>
       </c>
@@ -2923,7 +2939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1">
+    <row r="40" spans="1:12">
       <c r="A40" s="2">
         <v>44286</v>
       </c>
@@ -2961,7 +2977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1">
+    <row r="41" spans="1:12">
       <c r="A41" s="2">
         <v>44292</v>
       </c>
@@ -2999,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1">
+    <row r="42" spans="1:12">
       <c r="A42" s="2">
         <v>44292</v>
       </c>
@@ -3037,7 +3053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1">
+    <row r="43" spans="1:12">
       <c r="A43" s="2">
         <v>44293</v>
       </c>
@@ -3075,7 +3091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1">
+    <row r="44" spans="1:12">
       <c r="A44" s="2">
         <v>44293</v>
       </c>
@@ -3113,7 +3129,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1">
+    <row r="45" spans="1:12">
       <c r="A45" s="2">
         <v>44294</v>
       </c>
@@ -3151,7 +3167,7 @@
         <v>820.5</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1">
+    <row r="46" spans="1:12">
       <c r="A46" s="2">
         <v>44294</v>
       </c>
@@ -3189,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1">
+    <row r="47" spans="1:12">
       <c r="A47" s="2">
         <v>44294</v>
       </c>
@@ -3227,7 +3243,7 @@
         <v>244.5</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1">
+    <row r="48" spans="1:12">
       <c r="A48" s="2">
         <v>44295</v>
       </c>
@@ -3265,7 +3281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1">
+    <row r="49" spans="1:12">
       <c r="A49" s="2">
         <v>44295</v>
       </c>
@@ -3303,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1">
+    <row r="50" spans="1:12">
       <c r="A50" s="2">
         <v>44295</v>
       </c>
@@ -3341,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1">
+    <row r="51" spans="1:12">
       <c r="A51" s="2">
         <v>44298</v>
       </c>
@@ -3379,7 +3395,7 @@
         <v>808.5</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1">
+    <row r="52" spans="1:12">
       <c r="A52" s="2">
         <v>44299</v>
       </c>
@@ -3417,7 +3433,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1">
+    <row r="53" spans="1:12">
       <c r="A53" s="2">
         <v>44299</v>
       </c>
@@ -3455,7 +3471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1">
+    <row r="54" spans="1:12">
       <c r="A54" s="2">
         <v>44299</v>
       </c>
@@ -3493,7 +3509,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1">
+    <row r="55" spans="1:12">
       <c r="A55" s="2">
         <v>44299</v>
       </c>
@@ -3531,7 +3547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1">
+    <row r="56" spans="1:12">
       <c r="A56" s="2">
         <v>44299</v>
       </c>
@@ -3569,7 +3585,7 @@
         <v>439.5</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1">
+    <row r="57" spans="1:12">
       <c r="A57" s="2">
         <v>44300</v>
       </c>
@@ -3607,7 +3623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1">
+    <row r="58" spans="1:12">
       <c r="A58" s="2">
         <v>44300</v>
       </c>
@@ -3645,7 +3661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1">
+    <row r="59" spans="1:12">
       <c r="A59" s="2">
         <v>44300</v>
       </c>
@@ -3683,7 +3699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1">
+    <row r="60" spans="1:12">
       <c r="A60" s="2">
         <v>44301</v>
       </c>
@@ -3721,7 +3737,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1">
+    <row r="61" spans="1:12">
       <c r="A61" s="2">
         <v>44302</v>
       </c>
@@ -3759,7 +3775,7 @@
         <v>262.5</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1">
+    <row r="62" spans="1:12">
       <c r="A62" s="2">
         <v>44306</v>
       </c>
@@ -3797,7 +3813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1">
+    <row r="63" spans="1:12">
       <c r="A63" s="2">
         <v>44306</v>
       </c>
@@ -3835,7 +3851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1">
+    <row r="64" spans="1:12">
       <c r="A64" s="2">
         <v>44327</v>
       </c>
@@ -3873,7 +3889,7 @@
         <v>132.6</v>
       </c>
     </row>
-    <row r="65" spans="1:12" hidden="1">
+    <row r="65" spans="1:12">
       <c r="A65" s="2">
         <v>44327</v>
       </c>
@@ -3911,7 +3927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1">
+    <row r="66" spans="1:12">
       <c r="A66" s="2">
         <v>44327</v>
       </c>
@@ -3949,7 +3965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1">
+    <row r="67" spans="1:12">
       <c r="A67" s="2">
         <v>44327</v>
       </c>
@@ -3987,7 +4003,7 @@
         <v>132.6</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1">
+    <row r="68" spans="1:12">
       <c r="A68" s="2">
         <v>44327</v>
       </c>
@@ -4025,7 +4041,7 @@
         <v>132.6</v>
       </c>
     </row>
-    <row r="69" spans="1:12" hidden="1">
+    <row r="69" spans="1:12">
       <c r="A69" s="2">
         <v>44327</v>
       </c>
@@ -4063,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" hidden="1">
+    <row r="70" spans="1:12">
       <c r="A70" s="2">
         <v>44327</v>
       </c>
@@ -4101,7 +4117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1">
+    <row r="71" spans="1:12">
       <c r="A71" s="2">
         <v>44327</v>
       </c>
@@ -4139,7 +4155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1">
+    <row r="72" spans="1:12">
       <c r="A72" s="2">
         <v>44329</v>
       </c>
@@ -4177,7 +4193,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1">
+    <row r="73" spans="1:12">
       <c r="A73" s="2">
         <v>44329</v>
       </c>
@@ -4215,7 +4231,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1">
+    <row r="74" spans="1:12">
       <c r="A74" s="2">
         <v>44329</v>
       </c>
@@ -4253,7 +4269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1">
+    <row r="75" spans="1:12">
       <c r="A75" s="2">
         <v>44329</v>
       </c>
@@ -4291,7 +4307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" hidden="1">
+    <row r="76" spans="1:12">
       <c r="A76" s="2">
         <v>44329</v>
       </c>
@@ -4329,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" hidden="1">
+    <row r="77" spans="1:12">
       <c r="A77" s="2">
         <v>44329</v>
       </c>
@@ -4367,7 +4383,7 @@
         <v>349.5</v>
       </c>
     </row>
-    <row r="78" spans="1:12" hidden="1">
+    <row r="78" spans="1:12">
       <c r="A78" s="2">
         <v>44329</v>
       </c>
@@ -4405,7 +4421,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="79" spans="1:12" hidden="1">
+    <row r="79" spans="1:12">
       <c r="A79" s="2">
         <v>44330</v>
       </c>
@@ -4443,7 +4459,7 @@
         <v>209.1</v>
       </c>
     </row>
-    <row r="80" spans="1:12" hidden="1">
+    <row r="80" spans="1:12">
       <c r="A80" s="2">
         <v>44330</v>
       </c>
@@ -4481,7 +4497,7 @@
         <v>457.2</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1">
+    <row r="81" spans="1:12">
       <c r="A81" s="2">
         <v>44333</v>
       </c>
@@ -4519,7 +4535,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="82" spans="1:12" hidden="1">
+    <row r="82" spans="1:12">
       <c r="A82" s="2">
         <v>44334</v>
       </c>
@@ -4557,7 +4573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" hidden="1">
+    <row r="83" spans="1:12">
       <c r="A83" s="2">
         <v>44334</v>
       </c>
@@ -4595,7 +4611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" hidden="1">
+    <row r="84" spans="1:12">
       <c r="A84" s="2">
         <v>44337</v>
       </c>
@@ -4633,7 +4649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:12" hidden="1">
+    <row r="85" spans="1:12">
       <c r="A85" s="2">
         <v>44337</v>
       </c>
@@ -4671,7 +4687,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="86" spans="1:12" hidden="1">
+    <row r="86" spans="1:12">
       <c r="A86" s="2">
         <v>44399</v>
       </c>
@@ -4709,7 +4725,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="87" spans="1:12" hidden="1">
+    <row r="87" spans="1:12">
       <c r="A87" s="2">
         <v>44399</v>
       </c>
@@ -4747,7 +4763,7 @@
         <v>589.5</v>
       </c>
     </row>
-    <row r="88" spans="1:12" hidden="1">
+    <row r="88" spans="1:12">
       <c r="A88" s="2">
         <v>44406</v>
       </c>
@@ -4785,7 +4801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12" hidden="1">
+    <row r="89" spans="1:12">
       <c r="A89" s="2">
         <v>44407</v>
       </c>
@@ -4823,7 +4839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:12" hidden="1">
+    <row r="90" spans="1:12">
       <c r="A90" s="2">
         <v>44407</v>
       </c>
@@ -4861,7 +4877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:12" hidden="1">
+    <row r="91" spans="1:12">
       <c r="A91" s="2">
         <v>44407</v>
       </c>
@@ -4899,7 +4915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:12" hidden="1">
+    <row r="92" spans="1:12">
       <c r="A92" s="2">
         <v>44412</v>
       </c>
@@ -4937,7 +4953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:12" hidden="1">
+    <row r="93" spans="1:12">
       <c r="A93" s="2">
         <v>44412</v>
       </c>
@@ -4975,7 +4991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1">
+    <row r="94" spans="1:12">
       <c r="A94" s="2">
         <v>44412</v>
       </c>
@@ -5013,7 +5029,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="95" spans="1:12" hidden="1">
+    <row r="95" spans="1:12">
       <c r="A95" s="2">
         <v>44412</v>
       </c>
@@ -5051,7 +5067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:12" hidden="1">
+    <row r="96" spans="1:12">
       <c r="A96" s="2">
         <v>44412</v>
       </c>
@@ -5089,7 +5105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:12" hidden="1">
+    <row r="97" spans="1:12">
       <c r="A97" s="2">
         <v>44412</v>
       </c>
@@ -5127,7 +5143,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1">
+    <row r="98" spans="1:12">
       <c r="A98" s="2">
         <v>44412</v>
       </c>
@@ -5165,7 +5181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1">
+    <row r="99" spans="1:12">
       <c r="A99" s="2">
         <v>44412</v>
       </c>
@@ -5203,7 +5219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1">
+    <row r="100" spans="1:12">
       <c r="A100" s="2">
         <v>44412</v>
       </c>
@@ -5241,7 +5257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1">
+    <row r="101" spans="1:12">
       <c r="A101" s="2">
         <v>44412</v>
       </c>
@@ -5279,7 +5295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:12" hidden="1">
+    <row r="102" spans="1:12">
       <c r="A102" s="2">
         <v>44412</v>
       </c>
@@ -5317,7 +5333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1">
+    <row r="103" spans="1:12">
       <c r="A103" s="2">
         <v>44412</v>
       </c>
@@ -5355,7 +5371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1">
+    <row r="104" spans="1:12">
       <c r="A104" s="2">
         <v>44412</v>
       </c>
@@ -5393,7 +5409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:12" hidden="1">
+    <row r="105" spans="1:12">
       <c r="A105" s="2">
         <v>44412</v>
       </c>
@@ -5431,7 +5447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:12" hidden="1">
+    <row r="106" spans="1:12">
       <c r="A106" s="2">
         <v>44454</v>
       </c>
@@ -5469,7 +5485,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="107" spans="1:12" hidden="1">
+    <row r="107" spans="1:12">
       <c r="A107" s="2">
         <v>44454</v>
       </c>
@@ -5507,7 +5523,7 @@
         <v>255.9</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1">
+    <row r="108" spans="1:12">
       <c r="A108" s="2">
         <v>44462</v>
       </c>
@@ -5545,7 +5561,7 @@
         <v>352.5</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1">
+    <row r="109" spans="1:12">
       <c r="A109" s="2">
         <v>44462</v>
       </c>
@@ -5583,7 +5599,7 @@
         <v>355.5</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1">
+    <row r="110" spans="1:12">
       <c r="A110" s="2">
         <v>44462</v>
       </c>
@@ -5621,7 +5637,7 @@
         <v>1075.5</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1">
+    <row r="111" spans="1:12">
       <c r="A111" s="2">
         <v>44462</v>
       </c>
@@ -5659,7 +5675,7 @@
         <v>133.35</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1">
+    <row r="112" spans="1:12">
       <c r="A112" s="2">
         <v>44462</v>
       </c>
@@ -5697,7 +5713,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="113" spans="1:12" hidden="1">
+    <row r="113" spans="1:12">
       <c r="A113" s="2">
         <v>44462</v>
       </c>
@@ -5735,7 +5751,7 @@
         <v>134.55000000000001</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1">
+    <row r="114" spans="1:12">
       <c r="A114" s="2">
         <v>44466</v>
       </c>
@@ -5773,7 +5789,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1">
+    <row r="115" spans="1:12">
       <c r="A115" s="2">
         <v>44466</v>
       </c>
@@ -5811,7 +5827,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1">
+    <row r="116" spans="1:12">
       <c r="A116" s="2">
         <v>44473</v>
       </c>
@@ -5849,7 +5865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1">
+    <row r="117" spans="1:12">
       <c r="A117" s="2">
         <v>44481</v>
       </c>
@@ -5887,7 +5903,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1">
+    <row r="118" spans="1:12">
       <c r="A118" s="2">
         <v>44484</v>
       </c>
@@ -5925,7 +5941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1">
+    <row r="119" spans="1:12">
       <c r="A119" s="2">
         <v>44490</v>
       </c>
@@ -5963,7 +5979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:12" hidden="1">
+    <row r="120" spans="1:12">
       <c r="A120" s="2">
         <v>44495</v>
       </c>
@@ -6001,7 +6017,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1">
+    <row r="121" spans="1:12">
       <c r="A121" s="2">
         <v>44529</v>
       </c>
@@ -6039,7 +6055,7 @@
         <v>560.70000000000005</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1">
+    <row r="122" spans="1:12">
       <c r="A122" s="2">
         <v>44529</v>
       </c>
@@ -6077,7 +6093,7 @@
         <v>1791</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1">
+    <row r="123" spans="1:12">
       <c r="A123" s="2">
         <v>44530</v>
       </c>
@@ -6115,7 +6131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:12" hidden="1">
+    <row r="124" spans="1:12">
       <c r="A124" s="2">
         <v>44530</v>
       </c>
@@ -6153,7 +6169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12" hidden="1">
+    <row r="125" spans="1:12">
       <c r="A125" s="2">
         <v>44532</v>
       </c>
@@ -6191,7 +6207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1">
+    <row r="126" spans="1:12">
       <c r="A126" s="2">
         <v>44533</v>
       </c>
@@ -6229,7 +6245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:12" hidden="1">
+    <row r="127" spans="1:12">
       <c r="A127" s="2">
         <v>44553</v>
       </c>
@@ -6267,7 +6283,7 @@
         <v>150.9</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1">
+    <row r="128" spans="1:12">
       <c r="A128" s="2">
         <v>44554</v>
       </c>
@@ -6305,7 +6321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1">
+    <row r="129" spans="1:12">
       <c r="A129" s="2">
         <v>44557</v>
       </c>
@@ -6343,7 +6359,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1">
+    <row r="130" spans="1:12">
       <c r="A130" s="2">
         <v>44566</v>
       </c>
@@ -6381,7 +6397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1">
+    <row r="131" spans="1:12">
       <c r="A131" s="2">
         <v>44567</v>
       </c>
@@ -6419,7 +6435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1">
+    <row r="132" spans="1:12">
       <c r="A132" s="2">
         <v>44568</v>
       </c>
@@ -6457,7 +6473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1">
+    <row r="133" spans="1:12">
       <c r="A133" s="2">
         <v>44586</v>
       </c>
@@ -6495,7 +6511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:12" hidden="1">
+    <row r="134" spans="1:12">
       <c r="A134" s="2">
         <v>44587</v>
       </c>
@@ -6533,7 +6549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:12" hidden="1">
+    <row r="135" spans="1:12">
       <c r="A135" s="2">
         <v>44587</v>
       </c>
@@ -6571,7 +6587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:12" hidden="1">
+    <row r="136" spans="1:12">
       <c r="A136" s="2">
         <v>44624</v>
       </c>
@@ -6609,7 +6625,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="137" spans="1:12" hidden="1">
+    <row r="137" spans="1:12">
       <c r="A137" s="2">
         <v>44638</v>
       </c>
@@ -6647,7 +6663,7 @@
         <v>388.5</v>
       </c>
     </row>
-    <row r="138" spans="1:12" hidden="1">
+    <row r="138" spans="1:12">
       <c r="A138" s="2">
         <v>44644</v>
       </c>
@@ -6685,7 +6701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:12" hidden="1">
+    <row r="139" spans="1:12">
       <c r="A139" s="2">
         <v>44650</v>
       </c>
@@ -6723,7 +6739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:12" hidden="1">
+    <row r="140" spans="1:12">
       <c r="A140" s="2">
         <v>44652</v>
       </c>
@@ -6761,7 +6777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:12" hidden="1">
+    <row r="141" spans="1:12">
       <c r="A141" s="2">
         <v>44658</v>
       </c>
@@ -6799,7 +6815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:12" hidden="1">
+    <row r="142" spans="1:12">
       <c r="A142" s="2">
         <v>44753</v>
       </c>
@@ -6837,7 +6853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1">
+    <row r="143" spans="1:12">
       <c r="A143" s="2">
         <v>44753</v>
       </c>
@@ -6875,7 +6891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1">
+    <row r="144" spans="1:12">
       <c r="A144" s="2">
         <v>44812</v>
       </c>
@@ -6913,7 +6929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:12" hidden="1">
+    <row r="145" spans="1:12">
       <c r="A145" s="2">
         <v>44838</v>
       </c>
@@ -6951,7 +6967,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="146" spans="1:12" hidden="1">
+    <row r="146" spans="1:12">
       <c r="A146" s="2">
         <v>44848</v>
       </c>
@@ -6989,7 +7005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:12" hidden="1">
+    <row r="147" spans="1:12">
       <c r="A147" s="2">
         <v>44848</v>
       </c>
@@ -7027,7 +7043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:12" hidden="1">
+    <row r="148" spans="1:12">
       <c r="A148" s="2">
         <v>44883</v>
       </c>
@@ -7065,7 +7081,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="149" spans="1:12" hidden="1">
+    <row r="149" spans="1:12">
       <c r="A149" s="2">
         <v>44897</v>
       </c>
@@ -7103,7 +7119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:12" hidden="1">
+    <row r="150" spans="1:12">
       <c r="A150" s="2">
         <v>44900</v>
       </c>
@@ -7141,7 +7157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:12" hidden="1">
+    <row r="151" spans="1:12">
       <c r="A151" s="2">
         <v>44902</v>
       </c>
@@ -7179,7 +7195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:12" hidden="1">
+    <row r="152" spans="1:12">
       <c r="A152" s="2">
         <v>44902</v>
       </c>
@@ -7217,7 +7233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:12" hidden="1">
+    <row r="153" spans="1:12">
       <c r="A153" s="2">
         <v>45009</v>
       </c>
@@ -7255,7 +7271,7 @@
         <v>1567.5</v>
       </c>
     </row>
-    <row r="154" spans="1:12" hidden="1">
+    <row r="154" spans="1:12">
       <c r="A154" s="2">
         <v>45117</v>
       </c>
@@ -7293,7 +7309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:12" hidden="1">
+    <row r="155" spans="1:12">
       <c r="A155" s="2">
         <v>45120</v>
       </c>
@@ -7331,7 +7347,7 @@
         <v>1196.6400000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:12" hidden="1">
+    <row r="156" spans="1:12">
       <c r="A156" s="2">
         <v>45139</v>
       </c>
@@ -7369,7 +7385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:12" hidden="1">
+    <row r="157" spans="1:12">
       <c r="A157" s="2">
         <v>45148</v>
       </c>
@@ -7407,7 +7423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:12" hidden="1">
+    <row r="158" spans="1:12">
       <c r="A158" s="2">
         <v>45154</v>
       </c>
@@ -7445,7 +7461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:12" hidden="1">
+    <row r="159" spans="1:12">
       <c r="A159" s="2">
         <v>45160</v>
       </c>
@@ -7483,7 +7499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:12" hidden="1">
+    <row r="160" spans="1:12">
       <c r="A160" s="2">
         <v>45232</v>
       </c>
@@ -7521,7 +7537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:12" hidden="1">
+    <row r="161" spans="1:12">
       <c r="A161" s="2">
         <v>45263</v>
       </c>
@@ -7559,7 +7575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:12" hidden="1">
+    <row r="162" spans="1:12">
       <c r="A162" s="2">
         <v>45294</v>
       </c>
@@ -7597,7 +7613,7 @@
         <v>628.80000000000007</v>
       </c>
     </row>
-    <row r="163" spans="1:12" hidden="1">
+    <row r="163" spans="1:12">
       <c r="A163" s="2">
         <v>45310</v>
       </c>
@@ -7635,7 +7651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:12" hidden="1">
+    <row r="164" spans="1:12">
       <c r="A164" s="2">
         <v>45344</v>
       </c>
@@ -7673,7 +7689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:12" hidden="1">
+    <row r="165" spans="1:12">
       <c r="A165" s="2">
         <v>45362</v>
       </c>
@@ -7711,7 +7727,7 @@
         <v>1591.2</v>
       </c>
     </row>
-    <row r="166" spans="1:12" hidden="1">
+    <row r="166" spans="1:12">
       <c r="A166" s="2">
         <v>45363</v>
       </c>
@@ -7749,7 +7765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:12" hidden="1">
+    <row r="167" spans="1:12">
       <c r="A167" s="2">
         <v>45389</v>
       </c>
@@ -7787,7 +7803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:12" hidden="1">
+    <row r="168" spans="1:12">
       <c r="A168" s="2">
         <v>45389</v>
       </c>
@@ -7825,7 +7841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:12" hidden="1">
+    <row r="169" spans="1:12">
       <c r="A169" s="2">
         <v>45389</v>
       </c>
@@ -7863,7 +7879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:12" hidden="1">
+    <row r="170" spans="1:12">
       <c r="A170" s="2">
         <v>45389</v>
       </c>
@@ -7901,7 +7917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:12" hidden="1">
+    <row r="171" spans="1:12">
       <c r="A171" s="2">
         <v>45397</v>
       </c>
@@ -7939,7 +7955,7 @@
         <v>4830</v>
       </c>
     </row>
-    <row r="172" spans="1:12" hidden="1">
+    <row r="172" spans="1:12">
       <c r="A172" s="2">
         <v>45397</v>
       </c>
@@ -7977,7 +7993,7 @@
         <v>14490</v>
       </c>
     </row>
-    <row r="173" spans="1:12" hidden="1">
+    <row r="173" spans="1:12">
       <c r="A173" s="2">
         <v>45401</v>
       </c>
@@ -8015,7 +8031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:12" hidden="1">
+    <row r="174" spans="1:12">
       <c r="A174" s="2">
         <v>45405</v>
       </c>
@@ -8053,7 +8069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:12" hidden="1">
+    <row r="175" spans="1:12">
       <c r="A175" s="2">
         <v>45411</v>
       </c>
@@ -8091,7 +8107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:12" hidden="1">
+    <row r="176" spans="1:12">
       <c r="A176" s="2">
         <v>45412</v>
       </c>
@@ -8129,7 +8145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:12" hidden="1">
+    <row r="177" spans="1:12">
       <c r="A177" s="2">
         <v>45414</v>
       </c>
@@ -8167,7 +8183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:12" hidden="1">
+    <row r="178" spans="1:12">
       <c r="A178" s="2">
         <v>45418</v>
       </c>
@@ -8205,7 +8221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:12" hidden="1">
+    <row r="179" spans="1:12">
       <c r="A179" s="2">
         <v>45475</v>
       </c>
@@ -8281,7 +8297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:12" hidden="1">
+    <row r="181" spans="1:12">
       <c r="A181" s="2">
         <v>45475</v>
       </c>
@@ -8319,7 +8335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:12" hidden="1">
+    <row r="182" spans="1:12">
       <c r="A182" s="2">
         <v>45475</v>
       </c>
@@ -8433,7 +8449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:12" hidden="1">
+    <row r="185" spans="1:12">
       <c r="A185" s="2">
         <v>45476</v>
       </c>
@@ -8471,7 +8487,7 @@
         <v>406.5</v>
       </c>
     </row>
-    <row r="186" spans="1:12" hidden="1">
+    <row r="186" spans="1:12">
       <c r="A186" s="2">
         <v>45476</v>
       </c>
@@ -8509,7 +8525,7 @@
         <v>569.1</v>
       </c>
     </row>
-    <row r="187" spans="1:12" hidden="1">
+    <row r="187" spans="1:12">
       <c r="A187" s="2">
         <v>45476</v>
       </c>
@@ -8547,7 +8563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:12" hidden="1">
+    <row r="188" spans="1:12">
       <c r="A188" s="2">
         <v>45476</v>
       </c>
@@ -8585,7 +8601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:12" hidden="1">
+    <row r="189" spans="1:12">
       <c r="A189" s="2">
         <v>45488</v>
       </c>
@@ -8623,7 +8639,7 @@
         <v>24720</v>
       </c>
     </row>
-    <row r="190" spans="1:12" hidden="1">
+    <row r="190" spans="1:12">
       <c r="A190" s="2">
         <v>45489</v>
       </c>
@@ -8661,7 +8677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:12" hidden="1">
+    <row r="191" spans="1:12">
       <c r="A191" s="2">
         <v>45489</v>
       </c>
@@ -8699,7 +8715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:12" hidden="1">
+    <row r="192" spans="1:12">
       <c r="A192" s="2">
         <v>45489</v>
       </c>
@@ -8775,7 +8791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:12" hidden="1">
+    <row r="194" spans="1:12">
       <c r="A194" s="2">
         <v>45490</v>
       </c>
@@ -8813,7 +8829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:12" hidden="1">
+    <row r="195" spans="1:12">
       <c r="A195" s="2">
         <v>45490</v>
       </c>
@@ -8851,7 +8867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:12" hidden="1">
+    <row r="196" spans="1:12">
       <c r="A196" s="2">
         <v>45490</v>
       </c>
@@ -8889,7 +8905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:12" hidden="1">
+    <row r="197" spans="1:12">
       <c r="A197" s="2">
         <v>45490</v>
       </c>
@@ -8927,7 +8943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:12" hidden="1">
+    <row r="198" spans="1:12">
       <c r="A198" s="2">
         <v>45492</v>
       </c>
@@ -8965,7 +8981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:12" hidden="1">
+    <row r="199" spans="1:12">
       <c r="A199" s="2">
         <v>45492</v>
       </c>
@@ -9003,7 +9019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:12" hidden="1">
+    <row r="200" spans="1:12">
       <c r="A200" s="2">
         <v>45492</v>
       </c>
@@ -9041,7 +9057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:12" hidden="1">
+    <row r="201" spans="1:12">
       <c r="A201" s="2">
         <v>45506</v>
       </c>
@@ -9079,7 +9095,7 @@
         <v>534.29999999999995</v>
       </c>
     </row>
-    <row r="202" spans="1:12" hidden="1">
+    <row r="202" spans="1:12">
       <c r="A202" s="2">
         <v>45506</v>
       </c>
@@ -9117,7 +9133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:12" hidden="1">
+    <row r="203" spans="1:12">
       <c r="A203" s="2">
         <v>45506</v>
       </c>
@@ -9155,7 +9171,7 @@
         <v>488.55</v>
       </c>
     </row>
-    <row r="204" spans="1:12" hidden="1">
+    <row r="204" spans="1:12">
       <c r="A204" s="2">
         <v>45506</v>
       </c>
@@ -9193,7 +9209,7 @@
         <v>543.75</v>
       </c>
     </row>
-    <row r="205" spans="1:12" hidden="1">
+    <row r="205" spans="1:12">
       <c r="A205" s="2">
         <v>45506</v>
       </c>
@@ -9231,7 +9247,7 @@
         <v>137.85</v>
       </c>
     </row>
-    <row r="206" spans="1:12" hidden="1">
+    <row r="206" spans="1:12">
       <c r="A206" s="2">
         <v>45509</v>
       </c>
@@ -9269,7 +9285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:12" hidden="1">
+    <row r="207" spans="1:12">
       <c r="A207" s="2">
         <v>45510</v>
       </c>
@@ -9307,7 +9323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:12" hidden="1">
+    <row r="208" spans="1:12">
       <c r="A208" s="2">
         <v>45510</v>
       </c>
@@ -9345,7 +9361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:12" hidden="1">
+    <row r="209" spans="1:12">
       <c r="A209" s="2">
         <v>45511</v>
       </c>
@@ -9383,7 +9399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:12" hidden="1">
+    <row r="210" spans="1:12">
       <c r="A210" s="2">
         <v>45511</v>
       </c>
@@ -9421,7 +9437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:12" hidden="1">
+    <row r="211" spans="1:12">
       <c r="A211" s="2">
         <v>45511</v>
       </c>
@@ -9459,7 +9475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:12" hidden="1">
+    <row r="212" spans="1:12">
       <c r="A212" s="2">
         <v>45533</v>
       </c>
@@ -9497,7 +9513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:12" hidden="1">
+    <row r="213" spans="1:12">
       <c r="A213" s="2">
         <v>45533</v>
       </c>
@@ -9535,7 +9551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:12" hidden="1">
+    <row r="214" spans="1:12">
       <c r="A214" s="2">
         <v>45533</v>
       </c>
@@ -9573,7 +9589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:12" hidden="1">
+    <row r="215" spans="1:12">
       <c r="A215" s="2">
         <v>45533</v>
       </c>
@@ -9611,7 +9627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:12" hidden="1">
+    <row r="216" spans="1:12">
       <c r="A216" s="2">
         <v>45546</v>
       </c>
@@ -9649,7 +9665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:12" hidden="1">
+    <row r="217" spans="1:12">
       <c r="A217" s="2">
         <v>45546</v>
       </c>
@@ -9687,7 +9703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:12" hidden="1">
+    <row r="218" spans="1:12">
       <c r="A218" s="2">
         <v>45559</v>
       </c>
@@ -9725,7 +9741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:12" hidden="1">
+    <row r="219" spans="1:12">
       <c r="A219" s="2">
         <v>45581</v>
       </c>
@@ -9953,7 +9969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:12" hidden="1">
+    <row r="225" spans="1:12">
       <c r="A225" s="2">
         <v>45614</v>
       </c>
@@ -9991,7 +10007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:12" hidden="1">
+    <row r="226" spans="1:12">
       <c r="A226" s="2">
         <v>45645</v>
       </c>
@@ -10105,7 +10121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:12" hidden="1">
+    <row r="229" spans="1:12">
       <c r="A229" s="2">
         <v>45649</v>
       </c>
@@ -10257,7 +10273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:12" hidden="1">
+    <row r="233" spans="1:12">
       <c r="A233" s="2">
         <v>45691</v>
       </c>
@@ -10295,7 +10311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:12" hidden="1">
+    <row r="234" spans="1:12">
       <c r="A234" s="2">
         <v>45691</v>
       </c>
@@ -10333,7 +10349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:12" hidden="1">
+    <row r="235" spans="1:12">
       <c r="A235" s="2">
         <v>45691</v>
       </c>
@@ -10371,7 +10387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:12" hidden="1">
+    <row r="236" spans="1:12">
       <c r="A236" s="2">
         <v>45719</v>
       </c>
@@ -10599,7 +10615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:12" hidden="1">
+    <row r="242" spans="1:12">
       <c r="A242" s="2">
         <v>45727</v>
       </c>
@@ -10637,7 +10653,7 @@
         <v>2910</v>
       </c>
     </row>
-    <row r="243" spans="1:12" hidden="1">
+    <row r="243" spans="1:12">
       <c r="A243" s="2">
         <v>45747</v>
       </c>
@@ -10675,7 +10691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:12" hidden="1">
+    <row r="244" spans="1:12">
       <c r="A244" s="2">
         <v>45755</v>
       </c>
@@ -10713,7 +10729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:12" hidden="1">
+    <row r="245" spans="1:12">
       <c r="A245" s="2">
         <v>45758</v>
       </c>
@@ -10752,18 +10768,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M245" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="TSLA"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="8">
-      <filters>
-        <filter val="Joint"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M245" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10773,7 +10778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
+    <sheetView topLeftCell="A279" workbookViewId="0">
       <selection activeCell="A317" sqref="A317"/>
     </sheetView>
   </sheetViews>

</xml_diff>